<commit_message>
Drug molecule testing 26-31 acid name updated
</commit_message>
<xml_diff>
--- a/Code_And_Data/Dataset/DrugMoleculeTesting_ConstantTime.xlsx
+++ b/Code_And_Data/Dataset/DrugMoleculeTesting_ConstantTime.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri.sharepoint.com/sites/AIandChemistryPositionParticle-Ogrp/Shared Documents/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/upasanaroy/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D550606B-8E97-48FB-9980-D8B2CC7495A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E947595B-D452-4344-84FB-7DF2CEBB9909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="46">
   <si>
     <t>Acid (name)</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>Predicted_Yield</t>
-  </si>
-  <si>
-    <t>Experimental</t>
   </si>
   <si>
     <t>diethylglycine</t>
@@ -175,12 +172,15 @@
   <si>
     <t>4-aminobenzoic acid</t>
   </si>
+  <si>
+    <t>(S)-1-butylpiperidine-2-carboxylic acid</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,21 +217,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -338,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -387,9 +372,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,30 +712,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0284D173-9243-8145-8C4D-CC2D2BC9D4B7}">
-  <dimension ref="A1:N361"/>
+  <dimension ref="A1:M361"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21.95">
+    <row r="1" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -793,37 +775,34 @@
       <c r="M1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="20" t="s">
+    </row>
+    <row r="2" spans="1:13" ht="20" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="20.100000000000001">
-      <c r="A2" s="8" t="s">
+      <c r="B2" s="11">
+        <v>1</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="11">
-        <v>1</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="D2" s="13">
+        <v>1</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="D2" s="13">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="F2" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="13">
+        <v>2</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H2" s="13">
-        <v>2</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J2" s="13">
         <v>0.42</v>
@@ -838,33 +817,33 @@
         <v>67.104012287689599</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="20.100000000000001">
+    <row r="3" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="11">
-        <v>1</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="D3" s="13">
         <v>1</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" s="13">
         <v>1.3</v>
       </c>
       <c r="G3" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I3" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J3" s="13">
         <v>0.36</v>
@@ -879,33 +858,33 @@
         <v>87.153948742509058</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="20.100000000000001">
+    <row r="4" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="11">
-        <v>1</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="D4" s="13">
         <v>1</v>
       </c>
       <c r="E4" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13">
+        <v>1</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="13">
+        <v>2</v>
+      </c>
+      <c r="I4" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F4" s="13">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="13">
-        <v>2</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J4" s="13">
         <v>0.5</v>
@@ -920,33 +899,33 @@
         <v>97.896761643664533</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="20.100000000000001">
+    <row r="5" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="11">
-        <v>1</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="D5" s="13">
         <v>1</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F5" s="13">
         <v>1.2</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H5" s="13">
         <v>2</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" s="13">
         <v>0.15</v>
@@ -961,33 +940,33 @@
         <v>83.728924115531029</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="20.100000000000001">
+    <row r="6" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="11">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="11">
-        <v>1</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="D6" s="13">
         <v>1</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F6" s="13">
         <v>1.3</v>
       </c>
       <c r="G6" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="13">
+        <v>2</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H6" s="13">
-        <v>2</v>
-      </c>
-      <c r="I6" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J6" s="13">
         <v>0.5</v>
@@ -1002,33 +981,33 @@
         <v>88.737887485905802</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="20.100000000000001">
+    <row r="7" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="11">
+        <v>1</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="11">
-        <v>1</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
       <c r="D7" s="13">
         <v>1</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F7" s="13">
         <v>1.28</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H7" s="13">
         <v>2</v>
       </c>
       <c r="I7" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J7" s="13">
         <v>0.5</v>
@@ -1043,33 +1022,33 @@
         <v>72.359156594539144</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="20.100000000000001">
+    <row r="8" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="15">
+        <v>1</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="15">
-        <v>1</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>32</v>
-      </c>
       <c r="D8" s="13">
         <v>1</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F8" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G8" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="13">
+        <v>2</v>
+      </c>
+      <c r="I8" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H8" s="13">
-        <v>2</v>
-      </c>
-      <c r="I8" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J8" s="13">
         <v>0.42</v>
@@ -1084,33 +1063,33 @@
         <v>69.820997164740305</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="20.100000000000001">
+    <row r="9" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="15">
+        <v>1</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="15">
-        <v>1</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>32</v>
-      </c>
       <c r="D9" s="13">
         <v>1</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F9" s="13">
         <v>1.3</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9" s="13">
         <v>0.36</v>
@@ -1125,33 +1104,33 @@
         <v>84.220164768923553</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="20.100000000000001">
+    <row r="10" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="11">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="11">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D10" s="13">
         <v>1</v>
       </c>
       <c r="E10" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13">
+        <v>1</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="13">
+        <v>2</v>
+      </c>
+      <c r="I10" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F10" s="13">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="13">
-        <v>2</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J10" s="13">
         <v>0.5</v>
@@ -1166,33 +1145,33 @@
         <v>91.929076001959217</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="20.100000000000001">
+    <row r="11" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D11" s="13">
         <v>1</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="13">
         <v>1.2</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H11" s="13">
         <v>2</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J11" s="13">
         <v>0.15</v>
@@ -1207,33 +1186,33 @@
         <v>82.968937191378529</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="20.100000000000001">
+    <row r="12" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="11">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="11">
-        <v>1</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D12" s="13">
         <v>1</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="13">
         <v>1.3</v>
       </c>
       <c r="G12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H12" s="13">
+        <v>2</v>
+      </c>
+      <c r="I12" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H12" s="13">
-        <v>2</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J12" s="13">
         <v>0.5</v>
@@ -1248,33 +1227,33 @@
         <v>87.479063851206178</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="20.100000000000001">
+    <row r="13" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A13" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" s="11">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="11">
-        <v>1</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="D13" s="13">
         <v>1</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="13">
         <v>1.28</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13" s="13">
         <v>2</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J13" s="13">
         <v>0.5</v>
@@ -1289,33 +1268,33 @@
         <v>71.877381527625616</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="20.100000000000001">
+    <row r="14" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A14" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="11">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="11">
-        <v>1</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D14" s="13">
         <v>1</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F14" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="13">
+        <v>2</v>
+      </c>
+      <c r="I14" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H14" s="13">
-        <v>2</v>
-      </c>
-      <c r="I14" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J14" s="13">
         <v>0.42</v>
@@ -1330,33 +1309,33 @@
         <v>97.562970486487927</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="20.100000000000001">
+    <row r="15" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="11">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="11">
-        <v>1</v>
-      </c>
-      <c r="C15" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="13">
         <v>1</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F15" s="13">
         <v>1.3</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H15" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I15" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J15" s="13">
         <v>0.36</v>
@@ -1371,33 +1350,33 @@
         <v>78.010463855289444</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="20.100000000000001">
+    <row r="16" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="11">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B16" s="11">
-        <v>1</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D16" s="13">
         <v>1</v>
       </c>
       <c r="E16" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="13">
+        <v>1</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="13">
+        <v>2</v>
+      </c>
+      <c r="I16" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F16" s="13">
-        <v>1</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="13">
-        <v>2</v>
-      </c>
-      <c r="I16" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J16" s="13">
         <v>0.5</v>
@@ -1412,33 +1391,33 @@
         <v>95.04506917634869</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="20.100000000000001">
+    <row r="17" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="11">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="11">
-        <v>1</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D17" s="13">
         <v>1</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="13">
         <v>1.2</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="13">
         <v>2</v>
       </c>
       <c r="I17" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J17" s="13">
         <v>0.15</v>
@@ -1453,33 +1432,33 @@
         <v>88.789945937576391</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="21.95">
+    <row r="18" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="11">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B18" s="11">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D18" s="13">
         <v>1</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" s="13">
         <v>1.3</v>
       </c>
       <c r="G18" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="13">
+        <v>2</v>
+      </c>
+      <c r="I18" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H18" s="13">
-        <v>2</v>
-      </c>
-      <c r="I18" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J18" s="13">
         <v>0.5</v>
@@ -1493,37 +1472,34 @@
       <c r="M18" s="13">
         <v>89.784903473011497</v>
       </c>
-      <c r="N18" s="18">
-        <v>0.85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="21.95">
+    </row>
+    <row r="19" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="11">
-        <v>1</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>34</v>
-      </c>
       <c r="D19" s="13">
         <v>1</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F19" s="13">
         <v>1.28</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="13">
         <v>2</v>
       </c>
       <c r="I19" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J19" s="13">
         <v>0.5</v>
@@ -1537,37 +1513,34 @@
       <c r="M19" s="13">
         <v>89.261903860987147</v>
       </c>
-      <c r="N19" s="18">
-        <v>0.88</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="20.100000000000001">
+    </row>
+    <row r="20" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="10">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="10">
-        <v>1</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D20" s="13">
         <v>1</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F20" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G20" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="13">
+        <v>2</v>
+      </c>
+      <c r="I20" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H20" s="13">
-        <v>2</v>
-      </c>
-      <c r="I20" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J20" s="13">
         <v>0.42</v>
@@ -1582,33 +1555,33 @@
         <v>70.305148582035059</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="20.100000000000001">
+    <row r="21" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" s="10">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="10">
-        <v>1</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D21" s="13">
         <v>1</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F21" s="13">
         <v>1.3</v>
       </c>
       <c r="G21" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H21" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I21" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J21" s="13">
         <v>0.36</v>
@@ -1623,33 +1596,33 @@
         <v>81.85069994766917</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="20.100000000000001">
+    <row r="22" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A22" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" s="10">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="10">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D22" s="13">
         <v>1</v>
       </c>
       <c r="E22" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="13">
+        <v>1</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="13">
+        <v>2</v>
+      </c>
+      <c r="I22" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F22" s="13">
-        <v>1</v>
-      </c>
-      <c r="G22" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="13">
-        <v>2</v>
-      </c>
-      <c r="I22" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J22" s="13">
         <v>0.5</v>
@@ -1664,33 +1637,33 @@
         <v>79.703531648004173</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="20.100000000000001">
+    <row r="23" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="10">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B23" s="10">
-        <v>1</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D23" s="13">
         <v>1</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="13">
         <v>1.2</v>
       </c>
       <c r="G23" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H23" s="13">
         <v>2</v>
       </c>
       <c r="I23" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J23" s="13">
         <v>0.15</v>
@@ -1705,33 +1678,33 @@
         <v>83.368554564391602</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="20.100000000000001">
+    <row r="24" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" s="10">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B24" s="10">
-        <v>1</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D24" s="13">
         <v>1</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F24" s="13">
         <v>1.3</v>
       </c>
       <c r="G24" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H24" s="13">
+        <v>2</v>
+      </c>
+      <c r="I24" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H24" s="13">
-        <v>2</v>
-      </c>
-      <c r="I24" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J24" s="13">
         <v>0.5</v>
@@ -1746,33 +1719,33 @@
         <v>87.953918549858329</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="20.100000000000001">
+    <row r="25" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="10">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="10">
-        <v>1</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>36</v>
-      </c>
       <c r="D25" s="13">
         <v>1</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F25" s="13">
         <v>1.28</v>
       </c>
       <c r="G25" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H25" s="13">
         <v>2</v>
       </c>
       <c r="I25" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J25" s="13">
         <v>0.5</v>
@@ -1787,33 +1760,33 @@
         <v>74.567145182144969</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="20.100000000000001">
+    <row r="26" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B26" s="10">
         <v>1</v>
       </c>
       <c r="C26" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="13">
+        <v>1</v>
+      </c>
+      <c r="E26" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="D26" s="13">
-        <v>1</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="F26" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G26" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H26" s="13">
+        <v>2</v>
+      </c>
+      <c r="I26" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H26" s="13">
-        <v>2</v>
-      </c>
-      <c r="I26" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J26" s="13">
         <v>0.42</v>
@@ -1828,33 +1801,33 @@
         <v>69.714361068033796</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="20.100000000000001">
+    <row r="27" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B27" s="10">
         <v>1</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="13">
         <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F27" s="13">
         <v>1.3</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H27" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I27" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J27" s="13">
         <v>0.36</v>
@@ -1869,33 +1842,33 @@
         <v>79.2500133933397</v>
       </c>
     </row>
-    <row r="28" spans="1:14" ht="20.100000000000001">
+    <row r="28" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B28" s="10">
         <v>1</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="13">
         <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F28" s="13">
+        <v>1</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H28" s="13">
+        <v>2</v>
+      </c>
+      <c r="I28" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F28" s="13">
-        <v>1</v>
-      </c>
-      <c r="G28" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H28" s="13">
-        <v>2</v>
-      </c>
-      <c r="I28" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J28" s="13">
         <v>0.5</v>
@@ -1910,33 +1883,33 @@
         <v>79.073571850789023</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="20.100000000000001">
+    <row r="29" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A29" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B29" s="10">
         <v>1</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="13">
         <v>1</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="13">
         <v>1.2</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H29" s="13">
         <v>2</v>
       </c>
       <c r="I29" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J29" s="13">
         <v>0.15</v>
@@ -1951,33 +1924,33 @@
         <v>82.91386364728335</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="20.100000000000001">
+    <row r="30" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A30" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B30" s="10">
         <v>1</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" s="13">
         <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F30" s="13">
         <v>1.3</v>
       </c>
       <c r="G30" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H30" s="13">
+        <v>2</v>
+      </c>
+      <c r="I30" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H30" s="13">
-        <v>2</v>
-      </c>
-      <c r="I30" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J30" s="13">
         <v>0.5</v>
@@ -1992,33 +1965,33 @@
         <v>80.656844311376062</v>
       </c>
     </row>
-    <row r="31" spans="1:14" ht="20.100000000000001">
+    <row r="31" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A31" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B31" s="10">
         <v>1</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="13">
         <v>1</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F31" s="13">
         <v>1.28</v>
       </c>
       <c r="G31" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H31" s="13">
         <v>2</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J31" s="13">
         <v>0.5</v>
@@ -2033,33 +2006,33 @@
         <v>70.638253109269527</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="20.100000000000001">
+    <row r="32" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A32" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="10">
-        <v>1</v>
-      </c>
-      <c r="C32" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D32" s="13">
         <v>1</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F32" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H32" s="13">
+        <v>2</v>
+      </c>
+      <c r="I32" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H32" s="13">
-        <v>2</v>
-      </c>
-      <c r="I32" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J32" s="13">
         <v>0.42</v>
@@ -2074,33 +2047,33 @@
         <v>64.033956077610483</v>
       </c>
     </row>
-    <row r="33" spans="1:14" ht="20.100000000000001">
+    <row r="33" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B33" s="10">
+        <v>1</v>
+      </c>
+      <c r="C33" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="10">
-        <v>1</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D33" s="13">
         <v>1</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F33" s="13">
         <v>1.3</v>
       </c>
       <c r="G33" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H33" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I33" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J33" s="13">
         <v>0.36</v>
@@ -2115,33 +2088,33 @@
         <v>77.207716945067048</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="20.100000000000001">
+    <row r="34" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="10">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="10">
-        <v>1</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D34" s="13">
         <v>1</v>
       </c>
       <c r="E34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="13">
+        <v>1</v>
+      </c>
+      <c r="G34" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H34" s="13">
+        <v>2</v>
+      </c>
+      <c r="I34" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F34" s="13">
-        <v>1</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="13">
-        <v>2</v>
-      </c>
-      <c r="I34" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J34" s="13">
         <v>0.5</v>
@@ -2156,33 +2129,33 @@
         <v>76.657633218469442</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="20.100000000000001">
+    <row r="35" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="10">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B35" s="10">
-        <v>1</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D35" s="13">
         <v>1</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F35" s="13">
         <v>1.2</v>
       </c>
       <c r="G35" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H35" s="13">
         <v>2</v>
       </c>
       <c r="I35" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J35" s="13">
         <v>0.15</v>
@@ -2197,33 +2170,33 @@
         <v>76.769292517120562</v>
       </c>
     </row>
-    <row r="36" spans="1:14" ht="21.95">
+    <row r="36" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="10">
+        <v>1</v>
+      </c>
+      <c r="C36" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="10">
-        <v>1</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D36" s="13">
         <v>1</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F36" s="13">
         <v>1.3</v>
       </c>
       <c r="G36" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H36" s="13">
+        <v>2</v>
+      </c>
+      <c r="I36" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H36" s="13">
-        <v>2</v>
-      </c>
-      <c r="I36" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J36" s="13">
         <v>0.5</v>
@@ -2237,37 +2210,34 @@
       <c r="M36" s="13">
         <v>82.882374109084083</v>
       </c>
-      <c r="N36" s="19">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="21.95">
+    </row>
+    <row r="37" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
+      <c r="C37" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="10">
-        <v>1</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="D37" s="13">
         <v>1</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F37" s="13">
         <v>1.28</v>
       </c>
       <c r="G37" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H37" s="13">
         <v>2</v>
       </c>
       <c r="I37" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J37" s="13">
         <v>0.5</v>
@@ -2281,37 +2251,34 @@
       <c r="M37" s="13">
         <v>72.033989022067345</v>
       </c>
-      <c r="N37" s="19">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="21.95">
+    </row>
+    <row r="38" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A38" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="10">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="10">
-        <v>1</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D38" s="13">
         <v>1</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F38" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G38" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H38" s="13">
+        <v>2</v>
+      </c>
+      <c r="I38" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H38" s="13">
-        <v>2</v>
-      </c>
-      <c r="I38" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J38" s="13">
         <v>0.42</v>
@@ -2325,35 +2292,34 @@
       <c r="M38" s="13">
         <v>62.38408884937396</v>
       </c>
-      <c r="N38" s="19"/>
-    </row>
-    <row r="39" spans="1:14" ht="21.95">
+    </row>
+    <row r="39" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39" s="10">
+        <v>1</v>
+      </c>
+      <c r="C39" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="10">
-        <v>1</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D39" s="13">
         <v>1</v>
       </c>
       <c r="E39" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F39" s="13">
         <v>1.3</v>
       </c>
       <c r="G39" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H39" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I39" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J39" s="13">
         <v>0.36</v>
@@ -2367,35 +2333,34 @@
       <c r="M39" s="13">
         <v>79.974497362953784</v>
       </c>
-      <c r="N39" s="19"/>
-    </row>
-    <row r="40" spans="1:14" ht="21.95">
+    </row>
+    <row r="40" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A40" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="10">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="10">
-        <v>1</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D40" s="13">
         <v>1</v>
       </c>
       <c r="E40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F40" s="13">
+        <v>1</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H40" s="13">
+        <v>2</v>
+      </c>
+      <c r="I40" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F40" s="13">
-        <v>1</v>
-      </c>
-      <c r="G40" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H40" s="13">
-        <v>2</v>
-      </c>
-      <c r="I40" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J40" s="13">
         <v>0.5</v>
@@ -2409,35 +2374,34 @@
       <c r="M40" s="13">
         <v>75.823533045259296</v>
       </c>
-      <c r="N40" s="19"/>
-    </row>
-    <row r="41" spans="1:14" ht="21.95">
+    </row>
+    <row r="41" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A41" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="10">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="10">
-        <v>1</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D41" s="13">
         <v>1</v>
       </c>
       <c r="E41" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F41" s="13">
         <v>1.2</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H41" s="13">
         <v>2</v>
       </c>
       <c r="I41" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J41" s="13">
         <v>0.15</v>
@@ -2451,35 +2415,34 @@
       <c r="M41" s="13">
         <v>73.305745742297063</v>
       </c>
-      <c r="N41" s="19"/>
-    </row>
-    <row r="42" spans="1:14" ht="21.95">
+    </row>
+    <row r="42" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A42" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="10">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B42" s="10">
-        <v>1</v>
-      </c>
-      <c r="C42" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D42" s="13">
         <v>1</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F42" s="13">
         <v>1.3</v>
       </c>
       <c r="G42" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H42" s="13">
+        <v>2</v>
+      </c>
+      <c r="I42" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H42" s="13">
-        <v>2</v>
-      </c>
-      <c r="I42" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J42" s="13">
         <v>0.5</v>
@@ -2493,37 +2456,34 @@
       <c r="M42" s="13">
         <v>82.681400769506766</v>
       </c>
-      <c r="N42" s="19">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" ht="21.95">
+    </row>
+    <row r="43" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A43" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B43" s="10">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B43" s="10">
-        <v>1</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D43" s="13">
         <v>1</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F43" s="13">
         <v>1.28</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H43" s="13">
         <v>2</v>
       </c>
       <c r="I43" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J43" s="13">
         <v>0.5</v>
@@ -2537,37 +2497,34 @@
       <c r="M43" s="13">
         <v>73.061506297991741</v>
       </c>
-      <c r="N43" s="19">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="21.95">
+    </row>
+    <row r="44" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A44" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="10">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B44" s="10">
-        <v>1</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D44" s="13">
         <v>1</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F44" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G44" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H44" s="13">
+        <v>2</v>
+      </c>
+      <c r="I44" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H44" s="13">
-        <v>2</v>
-      </c>
-      <c r="I44" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J44" s="13">
         <v>0.42</v>
@@ -2581,35 +2538,34 @@
       <c r="M44" s="13">
         <v>67.407893291742965</v>
       </c>
-      <c r="N44" s="19"/>
-    </row>
-    <row r="45" spans="1:14" ht="21.95">
+    </row>
+    <row r="45" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A45" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="10">
+        <v>1</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B45" s="10">
-        <v>1</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D45" s="13">
         <v>1</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F45" s="13">
         <v>1.3</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H45" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I45" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J45" s="13">
         <v>0.36</v>
@@ -2623,35 +2579,34 @@
       <c r="M45" s="13">
         <v>79.6705180983611</v>
       </c>
-      <c r="N45" s="19"/>
-    </row>
-    <row r="46" spans="1:14" ht="21.95">
+    </row>
+    <row r="46" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A46" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" s="10">
+        <v>1</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="10">
-        <v>1</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D46" s="13">
         <v>1</v>
       </c>
       <c r="E46" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F46" s="13">
+        <v>1</v>
+      </c>
+      <c r="G46" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="13">
+        <v>2</v>
+      </c>
+      <c r="I46" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F46" s="13">
-        <v>1</v>
-      </c>
-      <c r="G46" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H46" s="13">
-        <v>2</v>
-      </c>
-      <c r="I46" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J46" s="13">
         <v>0.5</v>
@@ -2665,35 +2620,34 @@
       <c r="M46" s="13">
         <v>75.872719742658731</v>
       </c>
-      <c r="N46" s="19"/>
-    </row>
-    <row r="47" spans="1:14" ht="21.95">
+    </row>
+    <row r="47" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" s="10">
+        <v>1</v>
+      </c>
+      <c r="C47" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B47" s="10">
-        <v>1</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D47" s="13">
         <v>1</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F47" s="13">
         <v>1.2</v>
       </c>
       <c r="G47" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H47" s="13">
         <v>2</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J47" s="13">
         <v>0.15</v>
@@ -2707,35 +2661,34 @@
       <c r="M47" s="13">
         <v>68.29919749012754</v>
       </c>
-      <c r="N47" s="19"/>
-    </row>
-    <row r="48" spans="1:14" ht="21.95">
+    </row>
+    <row r="48" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B48" s="10">
+        <v>1</v>
+      </c>
+      <c r="C48" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B48" s="10">
-        <v>1</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D48" s="13">
         <v>1</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F48" s="13">
         <v>1.3</v>
       </c>
       <c r="G48" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H48" s="13">
+        <v>2</v>
+      </c>
+      <c r="I48" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H48" s="13">
-        <v>2</v>
-      </c>
-      <c r="I48" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J48" s="13">
         <v>0.5</v>
@@ -2749,37 +2702,34 @@
       <c r="M48" s="13">
         <v>83.281615150956696</v>
       </c>
-      <c r="N48" s="19">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" ht="21.95">
+    </row>
+    <row r="49" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="10">
+        <v>1</v>
+      </c>
+      <c r="C49" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B49" s="10">
-        <v>1</v>
-      </c>
-      <c r="C49" s="8" t="s">
-        <v>42</v>
-      </c>
       <c r="D49" s="13">
         <v>1</v>
       </c>
       <c r="E49" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F49" s="13">
         <v>1.28</v>
       </c>
       <c r="G49" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H49" s="13">
         <v>2</v>
       </c>
       <c r="I49" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J49" s="13">
         <v>0.5</v>
@@ -2793,37 +2743,34 @@
       <c r="M49" s="13">
         <v>73.154231001633178</v>
       </c>
-      <c r="N49" s="19">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="20.100000000000001">
+    </row>
+    <row r="50" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="10">
+        <v>1</v>
+      </c>
+      <c r="C50" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B50" s="10">
-        <v>1</v>
-      </c>
-      <c r="C50" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D50" s="13">
         <v>1</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F50" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G50" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H50" s="13">
+        <v>2</v>
+      </c>
+      <c r="I50" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H50" s="13">
-        <v>2</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J50" s="13">
         <v>0.42</v>
@@ -2838,33 +2785,33 @@
         <v>73.503009478488124</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="20.100000000000001">
+    <row r="51" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="10">
+        <v>1</v>
+      </c>
+      <c r="C51" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B51" s="10">
-        <v>1</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D51" s="13">
         <v>1</v>
       </c>
       <c r="E51" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F51" s="13">
         <v>1.3</v>
       </c>
       <c r="G51" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H51" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J51" s="13">
         <v>0.36</v>
@@ -2879,33 +2826,33 @@
         <v>78.068539144225056</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="20.100000000000001">
+    <row r="52" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="10">
+        <v>1</v>
+      </c>
+      <c r="C52" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B52" s="10">
-        <v>1</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D52" s="13">
         <v>1</v>
       </c>
       <c r="E52" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F52" s="13">
+        <v>1</v>
+      </c>
+      <c r="G52" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H52" s="13">
+        <v>2</v>
+      </c>
+      <c r="I52" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F52" s="13">
-        <v>1</v>
-      </c>
-      <c r="G52" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H52" s="13">
-        <v>2</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J52" s="13">
         <v>0.5</v>
@@ -2920,33 +2867,33 @@
         <v>76.480282351177664</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="20.100000000000001">
+    <row r="53" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="10">
+        <v>1</v>
+      </c>
+      <c r="C53" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B53" s="10">
-        <v>1</v>
-      </c>
-      <c r="C53" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D53" s="13">
         <v>1</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F53" s="13">
         <v>1.2</v>
       </c>
       <c r="G53" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H53" s="13">
         <v>2</v>
       </c>
       <c r="I53" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J53" s="13">
         <v>0.15</v>
@@ -2961,33 +2908,33 @@
         <v>71.538850890391217</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="20.100000000000001">
+    <row r="54" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="10">
+        <v>1</v>
+      </c>
+      <c r="C54" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B54" s="10">
-        <v>1</v>
-      </c>
-      <c r="C54" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D54" s="13">
         <v>1</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F54" s="13">
         <v>1.3</v>
       </c>
       <c r="G54" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H54" s="13">
+        <v>2</v>
+      </c>
+      <c r="I54" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H54" s="13">
-        <v>2</v>
-      </c>
-      <c r="I54" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J54" s="13">
         <v>0.5</v>
@@ -3002,33 +2949,33 @@
         <v>74.527842445287803</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="20.100000000000001">
+    <row r="55" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="10">
+        <v>1</v>
+      </c>
+      <c r="C55" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="B55" s="10">
-        <v>1</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>44</v>
-      </c>
       <c r="D55" s="13">
         <v>1</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F55" s="13">
         <v>1.28</v>
       </c>
       <c r="G55" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H55" s="13">
         <v>2</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J55" s="13">
         <v>0.5</v>
@@ -3043,33 +2990,33 @@
         <v>65.357729165322056</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="20.100000000000001">
+    <row r="56" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B56" s="10">
         <v>1</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="13">
+        <v>1</v>
+      </c>
+      <c r="E56" s="12" t="s">
         <v>15</v>
-      </c>
-      <c r="D56" s="13">
-        <v>1</v>
-      </c>
-      <c r="E56" s="12" t="s">
-        <v>16</v>
       </c>
       <c r="F56" s="13">
         <v>1.1000000000000001</v>
       </c>
       <c r="G56" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H56" s="13">
+        <v>2</v>
+      </c>
+      <c r="I56" s="12" t="s">
         <v>17</v>
-      </c>
-      <c r="H56" s="13">
-        <v>2</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>18</v>
       </c>
       <c r="J56" s="13">
         <v>0.42</v>
@@ -3084,33 +3031,33 @@
         <v>67.725676971665564</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="20.100000000000001">
+    <row r="57" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B57" s="10">
         <v>1</v>
       </c>
       <c r="C57" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D57" s="13">
         <v>1</v>
       </c>
       <c r="E57" s="12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F57" s="13">
         <v>1.3</v>
       </c>
       <c r="G57" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H57" s="13">
         <v>2.2000000000000002</v>
       </c>
       <c r="I57" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J57" s="13">
         <v>0.36</v>
@@ -3125,33 +3072,33 @@
         <v>82.431961231857699</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="20.100000000000001">
+    <row r="58" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A58" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B58" s="10">
         <v>1</v>
       </c>
       <c r="C58" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D58" s="13">
         <v>1</v>
       </c>
       <c r="E58" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F58" s="13">
+        <v>1</v>
+      </c>
+      <c r="G58" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H58" s="13">
+        <v>2</v>
+      </c>
+      <c r="I58" s="12" t="s">
         <v>22</v>
-      </c>
-      <c r="F58" s="13">
-        <v>1</v>
-      </c>
-      <c r="G58" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="H58" s="13">
-        <v>2</v>
-      </c>
-      <c r="I58" s="12" t="s">
-        <v>23</v>
       </c>
       <c r="J58" s="13">
         <v>0.5</v>
@@ -3166,33 +3113,33 @@
         <v>71.208828417603925</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="20.100000000000001">
+    <row r="59" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A59" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
       </c>
       <c r="C59" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59" s="13">
         <v>1</v>
       </c>
       <c r="E59" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F59" s="13">
         <v>1.2</v>
       </c>
       <c r="G59" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H59" s="13">
         <v>2</v>
       </c>
       <c r="I59" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J59" s="13">
         <v>0.15</v>
@@ -3207,33 +3154,33 @@
         <v>62.431846609585783</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="20.100000000000001">
+    <row r="60" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A60" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B60" s="10">
         <v>1</v>
       </c>
       <c r="C60" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D60" s="13">
         <v>1</v>
       </c>
       <c r="E60" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F60" s="13">
         <v>1.3</v>
       </c>
       <c r="G60" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H60" s="13">
+        <v>2</v>
+      </c>
+      <c r="I60" s="12" t="s">
         <v>27</v>
-      </c>
-      <c r="H60" s="13">
-        <v>2</v>
-      </c>
-      <c r="I60" s="12" t="s">
-        <v>28</v>
       </c>
       <c r="J60" s="13">
         <v>0.5</v>
@@ -3248,33 +3195,33 @@
         <v>83.643034988207361</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="20.100000000000001">
+    <row r="61" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A61" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B61" s="10">
         <v>1</v>
       </c>
       <c r="C61" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D61" s="13">
         <v>1</v>
       </c>
       <c r="E61" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F61" s="13">
         <v>1.28</v>
       </c>
       <c r="G61" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H61" s="13">
         <v>2</v>
       </c>
       <c r="I61" s="12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J61" s="13">
         <v>0.5</v>
@@ -3289,7 +3236,7 @@
         <v>73.117326748145842</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="20.100000000000001">
+    <row r="62" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="B62" s="10"/>
       <c r="C62" s="8"/>
@@ -3302,7 +3249,7 @@
       <c r="K62" s="13"/>
       <c r="L62" s="13"/>
     </row>
-    <row r="63" spans="1:14" ht="20.100000000000001">
+    <row r="63" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A63" s="8"/>
       <c r="C63" s="8"/>
       <c r="E63" s="12"/>
@@ -3314,7 +3261,7 @@
       <c r="K63" s="13"/>
       <c r="L63" s="13"/>
     </row>
-    <row r="64" spans="1:14" ht="20.100000000000001">
+    <row r="64" spans="1:13" ht="20" x14ac:dyDescent="0.2">
       <c r="A64" s="8"/>
       <c r="C64" s="8"/>
       <c r="E64" s="12"/>
@@ -3325,7 +3272,7 @@
       <c r="K64" s="13"/>
       <c r="L64" s="13"/>
     </row>
-    <row r="65" spans="1:12" ht="20.100000000000001">
+    <row r="65" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A65" s="8"/>
       <c r="C65" s="8"/>
       <c r="E65" s="12"/>
@@ -3334,7 +3281,7 @@
       <c r="K65" s="13"/>
       <c r="L65" s="13"/>
     </row>
-    <row r="66" spans="1:12" ht="20.100000000000001">
+    <row r="66" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A66" s="8"/>
       <c r="C66" s="8"/>
       <c r="E66" s="12"/>
@@ -3343,7 +3290,7 @@
       <c r="K66" s="13"/>
       <c r="L66" s="13"/>
     </row>
-    <row r="67" spans="1:12" ht="20.100000000000001">
+    <row r="67" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A67" s="8"/>
       <c r="C67" s="8"/>
       <c r="E67" s="12"/>
@@ -3351,7 +3298,7 @@
       <c r="K67" s="13"/>
       <c r="L67" s="13"/>
     </row>
-    <row r="68" spans="1:12" ht="20.100000000000001">
+    <row r="68" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A68" s="8"/>
       <c r="C68" s="8"/>
       <c r="E68" s="12"/>
@@ -3359,7 +3306,7 @@
       <c r="K68" s="13"/>
       <c r="L68" s="13"/>
     </row>
-    <row r="69" spans="1:12" ht="20.100000000000001">
+    <row r="69" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A69" s="8"/>
       <c r="C69" s="8"/>
       <c r="E69" s="12"/>
@@ -3367,7 +3314,7 @@
       <c r="K69" s="13"/>
       <c r="L69" s="13"/>
     </row>
-    <row r="70" spans="1:12" ht="20.100000000000001">
+    <row r="70" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A70" s="8"/>
       <c r="C70" s="8"/>
       <c r="E70" s="12"/>
@@ -3375,1063 +3322,1063 @@
       <c r="K70" s="13"/>
       <c r="L70" s="13"/>
     </row>
-    <row r="71" spans="1:12" ht="20.100000000000001">
+    <row r="71" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A71" s="8"/>
       <c r="C71" s="8"/>
       <c r="E71" s="12"/>
       <c r="K71" s="13"/>
       <c r="L71" s="13"/>
     </row>
-    <row r="72" spans="1:12" ht="20.100000000000001">
+    <row r="72" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A72" s="8"/>
       <c r="C72" s="8"/>
       <c r="E72" s="12"/>
       <c r="K72" s="13"/>
       <c r="L72" s="13"/>
     </row>
-    <row r="73" spans="1:12" ht="20.100000000000001">
+    <row r="73" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A73" s="8"/>
       <c r="C73" s="8"/>
       <c r="E73" s="12"/>
       <c r="K73" s="13"/>
       <c r="L73" s="13"/>
     </row>
-    <row r="74" spans="1:12" ht="20.100000000000001">
+    <row r="74" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A74" s="8"/>
       <c r="C74" s="8"/>
       <c r="E74" s="12"/>
       <c r="K74" s="13"/>
       <c r="L74" s="13"/>
     </row>
-    <row r="75" spans="1:12" ht="20.100000000000001">
+    <row r="75" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A75" s="8"/>
       <c r="C75" s="8"/>
       <c r="E75" s="12"/>
       <c r="K75" s="13"/>
       <c r="L75" s="13"/>
     </row>
-    <row r="76" spans="1:12" ht="20.100000000000001">
+    <row r="76" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A76" s="8"/>
       <c r="C76" s="8"/>
       <c r="E76" s="12"/>
       <c r="K76" s="13"/>
       <c r="L76" s="13"/>
     </row>
-    <row r="77" spans="1:12" ht="20.100000000000001">
+    <row r="77" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A77" s="8"/>
       <c r="C77" s="8"/>
       <c r="E77" s="12"/>
       <c r="K77" s="13"/>
       <c r="L77" s="13"/>
     </row>
-    <row r="78" spans="1:12" ht="20.100000000000001">
+    <row r="78" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A78" s="8"/>
       <c r="C78" s="8"/>
       <c r="E78" s="12"/>
       <c r="K78" s="13"/>
       <c r="L78" s="13"/>
     </row>
-    <row r="79" spans="1:12" ht="20.100000000000001">
+    <row r="79" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A79" s="8"/>
       <c r="C79" s="8"/>
       <c r="E79" s="12"/>
       <c r="K79" s="13"/>
       <c r="L79" s="13"/>
     </row>
-    <row r="80" spans="1:12" ht="20.100000000000001">
+    <row r="80" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A80" s="8"/>
       <c r="C80" s="8"/>
       <c r="E80" s="12"/>
       <c r="K80" s="13"/>
       <c r="L80" s="13"/>
     </row>
-    <row r="81" spans="1:12" ht="20.100000000000001">
+    <row r="81" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A81" s="8"/>
       <c r="C81" s="8"/>
       <c r="E81" s="12"/>
       <c r="K81" s="13"/>
       <c r="L81" s="13"/>
     </row>
-    <row r="82" spans="1:12" ht="20.100000000000001">
+    <row r="82" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A82" s="8"/>
       <c r="C82" s="8"/>
       <c r="E82" s="12"/>
       <c r="K82" s="13"/>
       <c r="L82" s="13"/>
     </row>
-    <row r="83" spans="1:12" ht="20.100000000000001">
+    <row r="83" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A83" s="8"/>
       <c r="C83" s="8"/>
       <c r="E83" s="12"/>
       <c r="K83" s="13"/>
       <c r="L83" s="13"/>
     </row>
-    <row r="84" spans="1:12" ht="20.100000000000001">
+    <row r="84" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A84" s="8"/>
       <c r="C84" s="8"/>
       <c r="E84" s="12"/>
       <c r="K84" s="13"/>
       <c r="L84" s="13"/>
     </row>
-    <row r="85" spans="1:12" ht="20.100000000000001">
+    <row r="85" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A85" s="8"/>
       <c r="C85" s="8"/>
       <c r="E85" s="12"/>
       <c r="K85" s="13"/>
       <c r="L85" s="13"/>
     </row>
-    <row r="86" spans="1:12" ht="20.100000000000001">
+    <row r="86" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A86" s="8"/>
       <c r="C86" s="8"/>
       <c r="E86" s="12"/>
       <c r="K86" s="13"/>
       <c r="L86" s="13"/>
     </row>
-    <row r="87" spans="1:12" ht="20.100000000000001">
+    <row r="87" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A87" s="8"/>
       <c r="E87" s="12"/>
       <c r="K87" s="13"/>
       <c r="L87" s="13"/>
     </row>
-    <row r="88" spans="1:12" ht="20.100000000000001">
+    <row r="88" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A88" s="8"/>
       <c r="E88" s="12"/>
       <c r="K88" s="13"/>
       <c r="L88" s="13"/>
     </row>
-    <row r="89" spans="1:12" ht="20.100000000000001">
+    <row r="89" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A89" s="8"/>
       <c r="E89" s="12"/>
       <c r="K89" s="13"/>
       <c r="L89" s="13"/>
     </row>
-    <row r="90" spans="1:12" ht="20.100000000000001">
+    <row r="90" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A90" s="8"/>
       <c r="E90" s="12"/>
       <c r="K90" s="13"/>
       <c r="L90" s="13"/>
     </row>
-    <row r="91" spans="1:12" ht="20.100000000000001">
+    <row r="91" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A91" s="8"/>
       <c r="E91" s="12"/>
       <c r="K91" s="13"/>
       <c r="L91" s="13"/>
     </row>
-    <row r="92" spans="1:12" ht="20.100000000000001">
+    <row r="92" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A92" s="8"/>
       <c r="E92" s="12"/>
       <c r="K92" s="13"/>
       <c r="L92" s="13"/>
     </row>
-    <row r="93" spans="1:12" ht="20.100000000000001">
+    <row r="93" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A93" s="8"/>
       <c r="E93" s="12"/>
       <c r="K93" s="13"/>
       <c r="L93" s="13"/>
     </row>
-    <row r="94" spans="1:12" ht="20.100000000000001">
+    <row r="94" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A94" s="8"/>
       <c r="E94" s="12"/>
       <c r="K94" s="13"/>
       <c r="L94" s="13"/>
     </row>
-    <row r="95" spans="1:12" ht="20.100000000000001">
+    <row r="95" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A95" s="8"/>
       <c r="E95" s="12"/>
       <c r="K95" s="13"/>
       <c r="L95" s="13"/>
     </row>
-    <row r="96" spans="1:12" ht="20.100000000000001">
+    <row r="96" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A96" s="8"/>
       <c r="E96" s="12"/>
       <c r="K96" s="13"/>
       <c r="L96" s="13"/>
     </row>
-    <row r="97" spans="1:12" ht="20.100000000000001">
+    <row r="97" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A97" s="8"/>
       <c r="E97" s="12"/>
       <c r="K97" s="13"/>
       <c r="L97" s="13"/>
     </row>
-    <row r="98" spans="1:12" ht="20.100000000000001">
+    <row r="98" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A98" s="8"/>
       <c r="E98" s="12"/>
       <c r="K98" s="13"/>
       <c r="L98" s="13"/>
     </row>
-    <row r="99" spans="1:12" ht="20.100000000000001">
+    <row r="99" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A99" s="8"/>
       <c r="E99" s="12"/>
       <c r="K99" s="13"/>
       <c r="L99" s="13"/>
     </row>
-    <row r="100" spans="1:12" ht="20.100000000000001">
+    <row r="100" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A100" s="8"/>
       <c r="E100" s="12"/>
       <c r="K100" s="13"/>
       <c r="L100" s="13"/>
     </row>
-    <row r="101" spans="1:12" ht="20.100000000000001">
+    <row r="101" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A101" s="8"/>
       <c r="E101" s="12"/>
       <c r="K101" s="13"/>
       <c r="L101" s="13"/>
     </row>
-    <row r="102" spans="1:12" ht="20.100000000000001">
+    <row r="102" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A102" s="8"/>
       <c r="E102" s="12"/>
       <c r="K102" s="13"/>
       <c r="L102" s="13"/>
     </row>
-    <row r="103" spans="1:12" ht="20.100000000000001">
+    <row r="103" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A103" s="8"/>
       <c r="E103" s="12"/>
       <c r="K103" s="13"/>
       <c r="L103" s="13"/>
     </row>
-    <row r="104" spans="1:12" ht="20.100000000000001">
+    <row r="104" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A104" s="8"/>
       <c r="E104" s="12"/>
       <c r="K104" s="13"/>
       <c r="L104" s="13"/>
     </row>
-    <row r="105" spans="1:12" ht="20.100000000000001">
+    <row r="105" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A105" s="8"/>
       <c r="E105" s="12"/>
       <c r="K105" s="13"/>
       <c r="L105" s="13"/>
     </row>
-    <row r="106" spans="1:12" ht="20.100000000000001">
+    <row r="106" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A106" s="8"/>
       <c r="E106" s="12"/>
       <c r="K106" s="13"/>
       <c r="L106" s="13"/>
     </row>
-    <row r="107" spans="1:12" ht="20.100000000000001">
+    <row r="107" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A107" s="8"/>
       <c r="E107" s="12"/>
       <c r="K107" s="13"/>
       <c r="L107" s="13"/>
     </row>
-    <row r="108" spans="1:12" ht="20.100000000000001">
+    <row r="108" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A108" s="8"/>
       <c r="E108" s="12"/>
       <c r="K108" s="13"/>
       <c r="L108" s="13"/>
     </row>
-    <row r="109" spans="1:12" ht="20.100000000000001">
+    <row r="109" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A109" s="8"/>
       <c r="E109" s="12"/>
       <c r="K109" s="13"/>
       <c r="L109" s="13"/>
     </row>
-    <row r="110" spans="1:12" ht="20.100000000000001">
+    <row r="110" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A110" s="8"/>
       <c r="E110" s="12"/>
       <c r="K110" s="13"/>
       <c r="L110" s="13"/>
     </row>
-    <row r="111" spans="1:12" ht="20.100000000000001">
+    <row r="111" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A111" s="8"/>
       <c r="E111" s="12"/>
       <c r="K111" s="13"/>
       <c r="L111" s="13"/>
     </row>
-    <row r="112" spans="1:12" ht="20.100000000000001">
+    <row r="112" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A112" s="8"/>
       <c r="E112" s="12"/>
       <c r="K112" s="13"/>
       <c r="L112" s="13"/>
     </row>
-    <row r="113" spans="1:12" ht="20.100000000000001">
+    <row r="113" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A113" s="8"/>
       <c r="E113" s="12"/>
       <c r="K113" s="13"/>
       <c r="L113" s="13"/>
     </row>
-    <row r="114" spans="1:12" ht="20.100000000000001">
+    <row r="114" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A114" s="8"/>
       <c r="E114" s="12"/>
       <c r="K114" s="13"/>
       <c r="L114" s="13"/>
     </row>
-    <row r="115" spans="1:12" ht="20.100000000000001">
+    <row r="115" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A115" s="8"/>
       <c r="E115" s="12"/>
       <c r="K115" s="13"/>
     </row>
-    <row r="116" spans="1:12" ht="20.100000000000001">
+    <row r="116" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A116" s="8"/>
       <c r="E116" s="12"/>
     </row>
-    <row r="117" spans="1:12" ht="20.100000000000001">
+    <row r="117" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A117" s="8"/>
       <c r="E117" s="12"/>
     </row>
-    <row r="118" spans="1:12" ht="20.100000000000001">
+    <row r="118" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A118" s="8"/>
       <c r="E118" s="12"/>
     </row>
-    <row r="119" spans="1:12" ht="20.100000000000001">
+    <row r="119" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A119" s="8"/>
       <c r="E119" s="12"/>
     </row>
-    <row r="120" spans="1:12" ht="20.100000000000001">
+    <row r="120" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A120" s="8"/>
       <c r="E120" s="12"/>
     </row>
-    <row r="121" spans="1:12" ht="20.100000000000001">
+    <row r="121" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A121" s="8"/>
       <c r="E121" s="12"/>
     </row>
-    <row r="122" spans="1:12" ht="20.100000000000001">
+    <row r="122" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A122" s="8"/>
       <c r="E122" s="12"/>
     </row>
-    <row r="123" spans="1:12" ht="20.100000000000001">
+    <row r="123" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A123" s="8"/>
       <c r="E123" s="12"/>
     </row>
-    <row r="124" spans="1:12" ht="20.100000000000001">
+    <row r="124" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A124" s="8"/>
       <c r="E124" s="12"/>
     </row>
-    <row r="125" spans="1:12" ht="20.100000000000001">
+    <row r="125" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A125" s="8"/>
       <c r="E125" s="12"/>
     </row>
-    <row r="126" spans="1:12" ht="20.100000000000001">
+    <row r="126" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A126" s="8"/>
       <c r="E126" s="12"/>
     </row>
-    <row r="127" spans="1:12" ht="20.100000000000001">
+    <row r="127" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A127" s="8"/>
       <c r="E127" s="12"/>
     </row>
-    <row r="128" spans="1:12" ht="20.100000000000001">
+    <row r="128" spans="1:12" ht="20" x14ac:dyDescent="0.2">
       <c r="A128" s="8"/>
       <c r="E128" s="12"/>
     </row>
-    <row r="129" spans="1:5" ht="20.100000000000001">
+    <row r="129" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A129" s="8"/>
       <c r="E129" s="12"/>
     </row>
-    <row r="130" spans="1:5" ht="20.100000000000001">
+    <row r="130" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A130" s="8"/>
       <c r="E130" s="12"/>
     </row>
-    <row r="131" spans="1:5" ht="20.100000000000001">
+    <row r="131" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A131" s="8"/>
       <c r="E131" s="12"/>
     </row>
-    <row r="132" spans="1:5" ht="20.100000000000001">
+    <row r="132" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A132" s="8"/>
       <c r="E132" s="12"/>
     </row>
-    <row r="133" spans="1:5" ht="20.100000000000001">
+    <row r="133" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A133" s="8"/>
       <c r="E133" s="12"/>
     </row>
-    <row r="134" spans="1:5" ht="20.100000000000001">
+    <row r="134" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A134" s="8"/>
       <c r="E134" s="12"/>
     </row>
-    <row r="135" spans="1:5" ht="20.100000000000001">
+    <row r="135" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A135" s="8"/>
       <c r="E135" s="12"/>
     </row>
-    <row r="136" spans="1:5" ht="20.100000000000001">
+    <row r="136" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A136" s="8"/>
       <c r="E136" s="12"/>
     </row>
-    <row r="137" spans="1:5" ht="20.100000000000001">
+    <row r="137" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A137" s="8"/>
       <c r="E137" s="12"/>
     </row>
-    <row r="138" spans="1:5" ht="20.100000000000001">
+    <row r="138" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A138" s="8"/>
       <c r="E138" s="12"/>
     </row>
-    <row r="139" spans="1:5" ht="20.100000000000001">
+    <row r="139" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A139" s="8"/>
       <c r="E139" s="12"/>
     </row>
-    <row r="140" spans="1:5" ht="20.100000000000001">
+    <row r="140" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A140" s="8"/>
       <c r="E140" s="12"/>
     </row>
-    <row r="141" spans="1:5" ht="20.100000000000001">
+    <row r="141" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A141" s="8"/>
       <c r="E141" s="12"/>
     </row>
-    <row r="142" spans="1:5" ht="20.100000000000001">
+    <row r="142" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A142" s="8"/>
       <c r="E142" s="12"/>
     </row>
-    <row r="143" spans="1:5" ht="20.100000000000001">
+    <row r="143" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A143" s="8"/>
       <c r="E143" s="12"/>
     </row>
-    <row r="144" spans="1:5" ht="20.100000000000001">
+    <row r="144" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A144" s="8"/>
       <c r="E144" s="12"/>
     </row>
-    <row r="145" spans="1:5" ht="20.100000000000001">
+    <row r="145" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A145" s="8"/>
       <c r="E145" s="12"/>
     </row>
-    <row r="146" spans="1:5" ht="20.100000000000001">
+    <row r="146" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A146" s="8"/>
       <c r="E146" s="12"/>
     </row>
-    <row r="147" spans="1:5" ht="20.100000000000001">
+    <row r="147" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A147" s="8"/>
       <c r="E147" s="12"/>
     </row>
-    <row r="148" spans="1:5" ht="20.100000000000001">
+    <row r="148" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A148" s="8"/>
       <c r="E148" s="12"/>
     </row>
-    <row r="149" spans="1:5" ht="20.100000000000001">
+    <row r="149" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A149" s="8"/>
       <c r="E149" s="12"/>
     </row>
-    <row r="150" spans="1:5" ht="20.100000000000001">
+    <row r="150" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A150" s="8"/>
       <c r="E150" s="12"/>
     </row>
-    <row r="151" spans="1:5" ht="20.100000000000001">
+    <row r="151" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A151" s="8"/>
       <c r="E151" s="12"/>
     </row>
-    <row r="152" spans="1:5" ht="20.100000000000001">
+    <row r="152" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A152" s="8"/>
     </row>
-    <row r="153" spans="1:5" ht="20.100000000000001">
+    <row r="153" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A153" s="8"/>
     </row>
-    <row r="154" spans="1:5" ht="20.100000000000001">
+    <row r="154" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A154" s="8"/>
     </row>
-    <row r="155" spans="1:5" ht="20.100000000000001">
+    <row r="155" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A155" s="8"/>
     </row>
-    <row r="156" spans="1:5" ht="20.100000000000001">
+    <row r="156" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A156" s="8"/>
     </row>
-    <row r="157" spans="1:5" ht="20.100000000000001">
+    <row r="157" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A157" s="8"/>
     </row>
-    <row r="158" spans="1:5" ht="20.100000000000001">
+    <row r="158" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A158" s="8"/>
     </row>
-    <row r="159" spans="1:5" ht="20.100000000000001">
+    <row r="159" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A159" s="8"/>
     </row>
-    <row r="160" spans="1:5" ht="20.100000000000001">
+    <row r="160" spans="1:5" ht="20" x14ac:dyDescent="0.2">
       <c r="A160" s="8"/>
     </row>
-    <row r="161" spans="1:1" ht="20.100000000000001">
+    <row r="161" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A161" s="8"/>
     </row>
-    <row r="162" spans="1:1" ht="20.100000000000001">
+    <row r="162" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A162" s="8"/>
     </row>
-    <row r="163" spans="1:1" ht="20.100000000000001">
+    <row r="163" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A163" s="8"/>
     </row>
-    <row r="164" spans="1:1" ht="20.100000000000001">
+    <row r="164" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A164" s="8"/>
     </row>
-    <row r="165" spans="1:1" ht="20.100000000000001">
+    <row r="165" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A165" s="8"/>
     </row>
-    <row r="166" spans="1:1" ht="20.100000000000001">
+    <row r="166" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A166" s="8"/>
     </row>
-    <row r="167" spans="1:1" ht="20.100000000000001">
+    <row r="167" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A167" s="8"/>
     </row>
-    <row r="168" spans="1:1" ht="20.100000000000001">
+    <row r="168" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A168" s="8"/>
     </row>
-    <row r="169" spans="1:1" ht="20.100000000000001">
+    <row r="169" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A169" s="8"/>
     </row>
-    <row r="170" spans="1:1" ht="20.100000000000001">
+    <row r="170" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A170" s="8"/>
     </row>
-    <row r="171" spans="1:1" ht="20.100000000000001">
+    <row r="171" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A171" s="8"/>
     </row>
-    <row r="172" spans="1:1" ht="20.100000000000001">
+    <row r="172" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A172" s="8"/>
     </row>
-    <row r="173" spans="1:1" ht="20.100000000000001">
+    <row r="173" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A173" s="8"/>
     </row>
-    <row r="174" spans="1:1" ht="20.100000000000001">
+    <row r="174" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A174" s="8"/>
     </row>
-    <row r="175" spans="1:1" ht="20.100000000000001">
+    <row r="175" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A175" s="8"/>
     </row>
-    <row r="176" spans="1:1" ht="20.100000000000001">
+    <row r="176" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A176" s="8"/>
     </row>
-    <row r="177" spans="1:1" ht="20.100000000000001">
+    <row r="177" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A177" s="8"/>
     </row>
-    <row r="178" spans="1:1" ht="20.100000000000001">
+    <row r="178" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A178" s="8"/>
     </row>
-    <row r="179" spans="1:1" ht="20.100000000000001">
+    <row r="179" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A179" s="8"/>
     </row>
-    <row r="180" spans="1:1" ht="20.100000000000001">
+    <row r="180" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A180" s="8"/>
     </row>
-    <row r="181" spans="1:1" ht="20.100000000000001">
+    <row r="181" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A181" s="8"/>
     </row>
-    <row r="182" spans="1:1" ht="20.100000000000001">
+    <row r="182" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A182" s="8"/>
     </row>
-    <row r="183" spans="1:1" ht="20.100000000000001">
+    <row r="183" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A183" s="8"/>
     </row>
-    <row r="184" spans="1:1" ht="20.100000000000001">
+    <row r="184" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A184" s="8"/>
     </row>
-    <row r="185" spans="1:1" ht="20.100000000000001">
+    <row r="185" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A185" s="8"/>
     </row>
-    <row r="186" spans="1:1" ht="20.100000000000001">
+    <row r="186" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A186" s="8"/>
     </row>
-    <row r="187" spans="1:1" ht="20.100000000000001">
+    <row r="187" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A187" s="8"/>
     </row>
-    <row r="188" spans="1:1" ht="20.100000000000001">
+    <row r="188" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A188" s="8"/>
     </row>
-    <row r="189" spans="1:1" ht="20.100000000000001">
+    <row r="189" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A189" s="8"/>
     </row>
-    <row r="190" spans="1:1" ht="20.100000000000001">
+    <row r="190" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A190" s="8"/>
     </row>
-    <row r="191" spans="1:1" ht="20.100000000000001">
+    <row r="191" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A191" s="8"/>
     </row>
-    <row r="192" spans="1:1" ht="20.100000000000001">
+    <row r="192" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A192" s="8"/>
     </row>
-    <row r="193" spans="1:1" ht="20.100000000000001">
+    <row r="193" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A193" s="8"/>
     </row>
-    <row r="194" spans="1:1" ht="20.100000000000001">
+    <row r="194" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A194" s="8"/>
     </row>
-    <row r="195" spans="1:1" ht="20.100000000000001">
+    <row r="195" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A195" s="8"/>
     </row>
-    <row r="196" spans="1:1" ht="20.100000000000001">
+    <row r="196" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A196" s="8"/>
     </row>
-    <row r="197" spans="1:1" ht="20.100000000000001">
+    <row r="197" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A197" s="8"/>
     </row>
-    <row r="198" spans="1:1" ht="20.100000000000001">
+    <row r="198" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A198" s="8"/>
     </row>
-    <row r="199" spans="1:1" ht="20.100000000000001">
+    <row r="199" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A199" s="8"/>
     </row>
-    <row r="200" spans="1:1" ht="20.100000000000001">
+    <row r="200" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A200" s="8"/>
     </row>
-    <row r="201" spans="1:1" ht="20.100000000000001">
+    <row r="201" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A201" s="8"/>
     </row>
-    <row r="202" spans="1:1" ht="20.100000000000001">
+    <row r="202" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A202" s="8"/>
     </row>
-    <row r="203" spans="1:1" ht="20.100000000000001">
+    <row r="203" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A203" s="8"/>
     </row>
-    <row r="204" spans="1:1" ht="20.100000000000001">
+    <row r="204" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A204" s="8"/>
     </row>
-    <row r="205" spans="1:1" ht="20.100000000000001">
+    <row r="205" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A205" s="8"/>
     </row>
-    <row r="206" spans="1:1" ht="20.100000000000001">
+    <row r="206" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A206" s="8"/>
     </row>
-    <row r="207" spans="1:1" ht="20.100000000000001">
+    <row r="207" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A207" s="8"/>
     </row>
-    <row r="208" spans="1:1" ht="20.100000000000001">
+    <row r="208" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A208" s="8"/>
     </row>
-    <row r="209" spans="1:1" ht="20.100000000000001">
+    <row r="209" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A209" s="8"/>
     </row>
-    <row r="210" spans="1:1" ht="20.100000000000001">
+    <row r="210" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A210" s="8"/>
     </row>
-    <row r="211" spans="1:1" ht="20.100000000000001">
+    <row r="211" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A211" s="8"/>
     </row>
-    <row r="212" spans="1:1" ht="20.100000000000001">
+    <row r="212" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A212" s="8"/>
     </row>
-    <row r="213" spans="1:1" ht="20.100000000000001">
+    <row r="213" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A213" s="8"/>
     </row>
-    <row r="214" spans="1:1" ht="20.100000000000001">
+    <row r="214" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A214" s="8"/>
     </row>
-    <row r="215" spans="1:1" ht="20.100000000000001">
+    <row r="215" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A215" s="8"/>
     </row>
-    <row r="216" spans="1:1" ht="20.100000000000001">
+    <row r="216" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A216" s="8"/>
     </row>
-    <row r="217" spans="1:1" ht="20.100000000000001">
+    <row r="217" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A217" s="8"/>
     </row>
-    <row r="218" spans="1:1" ht="20.100000000000001">
+    <row r="218" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A218" s="8"/>
     </row>
-    <row r="219" spans="1:1" ht="20.100000000000001">
+    <row r="219" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A219" s="8"/>
     </row>
-    <row r="220" spans="1:1" ht="20.100000000000001">
+    <row r="220" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A220" s="8"/>
     </row>
-    <row r="221" spans="1:1" ht="20.100000000000001">
+    <row r="221" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A221" s="8"/>
     </row>
-    <row r="222" spans="1:1" ht="20.100000000000001">
+    <row r="222" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A222" s="8"/>
     </row>
-    <row r="223" spans="1:1" ht="20.100000000000001">
+    <row r="223" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A223" s="8"/>
     </row>
-    <row r="224" spans="1:1" ht="20.100000000000001">
+    <row r="224" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A224" s="8"/>
     </row>
-    <row r="225" spans="1:1" ht="20.100000000000001">
+    <row r="225" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A225" s="8"/>
     </row>
-    <row r="226" spans="1:1" ht="20.100000000000001">
+    <row r="226" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A226" s="8"/>
     </row>
-    <row r="227" spans="1:1" ht="20.100000000000001">
+    <row r="227" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A227" s="8"/>
     </row>
-    <row r="228" spans="1:1" ht="20.100000000000001">
+    <row r="228" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A228" s="8"/>
     </row>
-    <row r="229" spans="1:1" ht="20.100000000000001">
+    <row r="229" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A229" s="8"/>
     </row>
-    <row r="230" spans="1:1" ht="20.100000000000001">
+    <row r="230" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A230" s="8"/>
     </row>
-    <row r="231" spans="1:1" ht="20.100000000000001">
+    <row r="231" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A231" s="8"/>
     </row>
-    <row r="232" spans="1:1" ht="20.100000000000001">
+    <row r="232" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A232" s="8"/>
     </row>
-    <row r="233" spans="1:1" ht="20.100000000000001">
+    <row r="233" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A233" s="8"/>
     </row>
-    <row r="234" spans="1:1" ht="20.100000000000001">
+    <row r="234" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A234" s="8"/>
     </row>
-    <row r="235" spans="1:1" ht="20.100000000000001">
+    <row r="235" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A235" s="8"/>
     </row>
-    <row r="236" spans="1:1" ht="20.100000000000001">
+    <row r="236" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A236" s="8"/>
     </row>
-    <row r="237" spans="1:1" ht="20.100000000000001">
+    <row r="237" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A237" s="8"/>
     </row>
-    <row r="238" spans="1:1" ht="20.100000000000001">
+    <row r="238" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A238" s="8"/>
     </row>
-    <row r="239" spans="1:1" ht="20.100000000000001">
+    <row r="239" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A239" s="8"/>
     </row>
-    <row r="240" spans="1:1" ht="20.100000000000001">
+    <row r="240" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A240" s="8"/>
     </row>
-    <row r="241" spans="1:1" ht="20.100000000000001">
+    <row r="241" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A241" s="8"/>
     </row>
-    <row r="242" spans="1:1" ht="20.100000000000001">
+    <row r="242" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A242" s="8"/>
     </row>
-    <row r="243" spans="1:1" ht="20.100000000000001">
+    <row r="243" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A243" s="8"/>
     </row>
-    <row r="244" spans="1:1" ht="20.100000000000001">
+    <row r="244" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A244" s="8"/>
     </row>
-    <row r="245" spans="1:1" ht="20.100000000000001">
+    <row r="245" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A245" s="8"/>
     </row>
-    <row r="246" spans="1:1" ht="20.100000000000001">
+    <row r="246" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A246" s="8"/>
     </row>
-    <row r="247" spans="1:1" ht="20.100000000000001">
+    <row r="247" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A247" s="8"/>
     </row>
-    <row r="248" spans="1:1" ht="20.100000000000001">
+    <row r="248" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A248" s="8"/>
     </row>
-    <row r="249" spans="1:1" ht="20.100000000000001">
+    <row r="249" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A249" s="8"/>
     </row>
-    <row r="250" spans="1:1" ht="20.100000000000001">
+    <row r="250" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A250" s="8"/>
     </row>
-    <row r="251" spans="1:1" ht="20.100000000000001">
+    <row r="251" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A251" s="8"/>
     </row>
-    <row r="252" spans="1:1" ht="20.100000000000001">
+    <row r="252" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A252" s="8"/>
     </row>
-    <row r="253" spans="1:1" ht="20.100000000000001">
+    <row r="253" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A253" s="8"/>
     </row>
-    <row r="254" spans="1:1" ht="20.100000000000001">
+    <row r="254" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A254" s="8"/>
     </row>
-    <row r="255" spans="1:1" ht="20.100000000000001">
+    <row r="255" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A255" s="8"/>
     </row>
-    <row r="256" spans="1:1" ht="20.100000000000001">
+    <row r="256" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A256" s="8"/>
     </row>
-    <row r="257" spans="1:1" ht="20.100000000000001">
+    <row r="257" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A257" s="8"/>
     </row>
-    <row r="258" spans="1:1" ht="20.100000000000001">
+    <row r="258" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A258" s="8"/>
     </row>
-    <row r="259" spans="1:1" ht="20.100000000000001">
+    <row r="259" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A259" s="8"/>
     </row>
-    <row r="260" spans="1:1" ht="20.100000000000001">
+    <row r="260" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A260" s="8"/>
     </row>
-    <row r="261" spans="1:1" ht="20.100000000000001">
+    <row r="261" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A261" s="8"/>
     </row>
-    <row r="262" spans="1:1" ht="20.100000000000001">
+    <row r="262" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A262" s="8"/>
     </row>
-    <row r="263" spans="1:1" ht="20.100000000000001">
+    <row r="263" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A263" s="8"/>
     </row>
-    <row r="264" spans="1:1" ht="20.100000000000001">
+    <row r="264" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A264" s="8"/>
     </row>
-    <row r="265" spans="1:1" ht="20.100000000000001">
+    <row r="265" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A265" s="8"/>
     </row>
-    <row r="266" spans="1:1" ht="20.100000000000001">
+    <row r="266" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A266" s="8"/>
     </row>
-    <row r="267" spans="1:1" ht="20.100000000000001">
+    <row r="267" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A267" s="8"/>
     </row>
-    <row r="268" spans="1:1" ht="20.100000000000001">
+    <row r="268" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A268" s="8"/>
     </row>
-    <row r="269" spans="1:1" ht="20.100000000000001">
+    <row r="269" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A269" s="8"/>
     </row>
-    <row r="270" spans="1:1" ht="20.100000000000001">
+    <row r="270" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A270" s="8"/>
     </row>
-    <row r="271" spans="1:1" ht="20.100000000000001">
+    <row r="271" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A271" s="8"/>
     </row>
-    <row r="272" spans="1:1" ht="20.100000000000001">
+    <row r="272" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A272" s="8"/>
     </row>
-    <row r="273" spans="1:1" ht="20.100000000000001">
+    <row r="273" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A273" s="8"/>
     </row>
-    <row r="274" spans="1:1" ht="20.100000000000001">
+    <row r="274" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A274" s="8"/>
     </row>
-    <row r="275" spans="1:1" ht="20.100000000000001">
+    <row r="275" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A275" s="8"/>
     </row>
-    <row r="276" spans="1:1" ht="20.100000000000001">
+    <row r="276" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A276" s="8"/>
     </row>
-    <row r="277" spans="1:1" ht="20.100000000000001">
+    <row r="277" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A277" s="8"/>
     </row>
-    <row r="278" spans="1:1" ht="20.100000000000001">
+    <row r="278" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A278" s="8"/>
     </row>
-    <row r="279" spans="1:1" ht="20.100000000000001">
+    <row r="279" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A279" s="8"/>
     </row>
-    <row r="280" spans="1:1" ht="20.100000000000001">
+    <row r="280" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A280" s="8"/>
     </row>
-    <row r="281" spans="1:1" ht="20.100000000000001">
+    <row r="281" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A281" s="8"/>
     </row>
-    <row r="282" spans="1:1" ht="20.100000000000001">
+    <row r="282" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A282" s="8"/>
     </row>
-    <row r="283" spans="1:1" ht="20.100000000000001">
+    <row r="283" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A283" s="8"/>
     </row>
-    <row r="284" spans="1:1" ht="20.100000000000001">
+    <row r="284" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A284" s="8"/>
     </row>
-    <row r="285" spans="1:1" ht="20.100000000000001">
+    <row r="285" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A285" s="8"/>
     </row>
-    <row r="286" spans="1:1" ht="20.100000000000001">
+    <row r="286" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A286" s="8"/>
     </row>
-    <row r="287" spans="1:1" ht="20.100000000000001">
+    <row r="287" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A287" s="8"/>
     </row>
-    <row r="288" spans="1:1" ht="20.100000000000001">
+    <row r="288" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A288" s="8"/>
     </row>
-    <row r="289" spans="1:1" ht="20.100000000000001">
+    <row r="289" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A289" s="8"/>
     </row>
-    <row r="290" spans="1:1" ht="20.100000000000001">
+    <row r="290" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A290" s="8"/>
     </row>
-    <row r="291" spans="1:1" ht="20.100000000000001">
+    <row r="291" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A291" s="8"/>
     </row>
-    <row r="292" spans="1:1" ht="20.100000000000001">
+    <row r="292" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A292" s="8"/>
     </row>
-    <row r="293" spans="1:1" ht="20.100000000000001">
+    <row r="293" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A293" s="8"/>
     </row>
-    <row r="294" spans="1:1" ht="20.100000000000001">
+    <row r="294" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A294" s="8"/>
     </row>
-    <row r="295" spans="1:1" ht="20.100000000000001">
+    <row r="295" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A295" s="8"/>
     </row>
-    <row r="296" spans="1:1" ht="20.100000000000001">
+    <row r="296" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A296" s="8"/>
     </row>
-    <row r="297" spans="1:1" ht="20.100000000000001">
+    <row r="297" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A297" s="8"/>
     </row>
-    <row r="298" spans="1:1" ht="20.100000000000001">
+    <row r="298" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A298" s="8"/>
     </row>
-    <row r="299" spans="1:1" ht="20.100000000000001">
+    <row r="299" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A299" s="8"/>
     </row>
-    <row r="300" spans="1:1" ht="20.100000000000001">
+    <row r="300" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A300" s="8"/>
     </row>
-    <row r="301" spans="1:1" ht="20.100000000000001">
+    <row r="301" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A301" s="8"/>
     </row>
-    <row r="302" spans="1:1" ht="20.100000000000001">
+    <row r="302" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A302" s="8"/>
     </row>
-    <row r="303" spans="1:1" ht="20.100000000000001">
+    <row r="303" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A303" s="8"/>
     </row>
-    <row r="304" spans="1:1" ht="20.100000000000001">
+    <row r="304" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A304" s="8"/>
     </row>
-    <row r="305" spans="1:1" ht="20.100000000000001">
+    <row r="305" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A305" s="8"/>
     </row>
-    <row r="306" spans="1:1" ht="20.100000000000001">
+    <row r="306" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A306" s="8"/>
     </row>
-    <row r="307" spans="1:1" ht="20.100000000000001">
+    <row r="307" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A307" s="8"/>
     </row>
-    <row r="308" spans="1:1" ht="20.100000000000001">
+    <row r="308" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A308" s="8"/>
     </row>
-    <row r="309" spans="1:1" ht="20.100000000000001">
+    <row r="309" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A309" s="8"/>
     </row>
-    <row r="310" spans="1:1" ht="20.100000000000001">
+    <row r="310" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A310" s="8"/>
     </row>
-    <row r="311" spans="1:1" ht="20.100000000000001">
+    <row r="311" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A311" s="8"/>
     </row>
-    <row r="312" spans="1:1" ht="20.100000000000001">
+    <row r="312" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A312" s="8"/>
     </row>
-    <row r="313" spans="1:1" ht="20.100000000000001">
+    <row r="313" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A313" s="8"/>
     </row>
-    <row r="314" spans="1:1" ht="20.100000000000001">
+    <row r="314" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A314" s="8"/>
     </row>
-    <row r="315" spans="1:1" ht="20.100000000000001">
+    <row r="315" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A315" s="8"/>
     </row>
-    <row r="316" spans="1:1" ht="20.100000000000001">
+    <row r="316" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A316" s="8"/>
     </row>
-    <row r="317" spans="1:1" ht="20.100000000000001">
+    <row r="317" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A317" s="8"/>
     </row>
-    <row r="318" spans="1:1" ht="20.100000000000001">
+    <row r="318" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A318" s="8"/>
     </row>
-    <row r="319" spans="1:1" ht="20.100000000000001">
+    <row r="319" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A319" s="8"/>
     </row>
-    <row r="320" spans="1:1" ht="20.100000000000001">
+    <row r="320" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A320" s="8"/>
     </row>
-    <row r="321" spans="1:1" ht="20.100000000000001">
+    <row r="321" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A321" s="8"/>
     </row>
-    <row r="322" spans="1:1" ht="20.100000000000001">
+    <row r="322" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A322" s="8"/>
     </row>
-    <row r="323" spans="1:1" ht="20.100000000000001">
+    <row r="323" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A323" s="8"/>
     </row>
-    <row r="324" spans="1:1" ht="20.100000000000001">
+    <row r="324" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A324" s="8"/>
     </row>
-    <row r="325" spans="1:1" ht="20.100000000000001">
+    <row r="325" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A325" s="8"/>
     </row>
-    <row r="326" spans="1:1" ht="20.100000000000001">
+    <row r="326" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A326" s="8"/>
     </row>
-    <row r="327" spans="1:1" ht="20.100000000000001">
+    <row r="327" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A327" s="8"/>
     </row>
-    <row r="328" spans="1:1" ht="20.100000000000001">
+    <row r="328" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A328" s="8"/>
     </row>
-    <row r="329" spans="1:1" ht="20.100000000000001">
+    <row r="329" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A329" s="8"/>
     </row>
-    <row r="330" spans="1:1" ht="20.100000000000001">
+    <row r="330" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A330" s="8"/>
     </row>
-    <row r="331" spans="1:1" ht="20.100000000000001">
+    <row r="331" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A331" s="8"/>
     </row>
-    <row r="332" spans="1:1" ht="20.100000000000001">
+    <row r="332" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A332" s="8"/>
     </row>
-    <row r="333" spans="1:1" ht="20.100000000000001">
+    <row r="333" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A333" s="8"/>
     </row>
-    <row r="334" spans="1:1" ht="20.100000000000001">
+    <row r="334" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A334" s="8"/>
     </row>
-    <row r="335" spans="1:1" ht="20.100000000000001">
+    <row r="335" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A335" s="8"/>
     </row>
-    <row r="336" spans="1:1" ht="20.100000000000001">
+    <row r="336" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A336" s="8"/>
     </row>
-    <row r="337" spans="1:1" ht="20.100000000000001">
+    <row r="337" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A337" s="8"/>
     </row>
-    <row r="338" spans="1:1" ht="20.100000000000001">
+    <row r="338" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A338" s="8"/>
     </row>
-    <row r="339" spans="1:1" ht="20.100000000000001">
+    <row r="339" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A339" s="8"/>
     </row>
-    <row r="340" spans="1:1" ht="20.100000000000001">
+    <row r="340" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A340" s="8"/>
     </row>
-    <row r="341" spans="1:1" ht="20.100000000000001">
+    <row r="341" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A341" s="8"/>
     </row>
-    <row r="342" spans="1:1" ht="20.100000000000001">
+    <row r="342" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A342" s="8"/>
     </row>
-    <row r="343" spans="1:1" ht="20.100000000000001">
+    <row r="343" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A343" s="8"/>
     </row>
-    <row r="344" spans="1:1" ht="20.100000000000001">
+    <row r="344" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A344" s="8"/>
     </row>
-    <row r="345" spans="1:1" ht="20.100000000000001">
+    <row r="345" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A345" s="8"/>
     </row>
-    <row r="346" spans="1:1" ht="20.100000000000001">
+    <row r="346" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A346" s="8"/>
     </row>
-    <row r="347" spans="1:1" ht="20.100000000000001">
+    <row r="347" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A347" s="8"/>
     </row>
-    <row r="348" spans="1:1" ht="20.100000000000001">
+    <row r="348" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A348" s="8"/>
     </row>
-    <row r="349" spans="1:1" ht="20.100000000000001">
+    <row r="349" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A349" s="8"/>
     </row>
-    <row r="350" spans="1:1" ht="20.100000000000001">
+    <row r="350" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A350" s="8"/>
     </row>
-    <row r="351" spans="1:1" ht="20.100000000000001">
+    <row r="351" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A351" s="8"/>
     </row>
-    <row r="352" spans="1:1" ht="20.100000000000001">
+    <row r="352" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A352" s="8"/>
     </row>
-    <row r="353" spans="1:1" ht="20.100000000000001">
+    <row r="353" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A353" s="8"/>
     </row>
-    <row r="354" spans="1:1" ht="20.100000000000001">
+    <row r="354" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A354" s="8"/>
     </row>
-    <row r="355" spans="1:1" ht="20.100000000000001">
+    <row r="355" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A355" s="8"/>
     </row>
-    <row r="356" spans="1:1" ht="20.100000000000001">
+    <row r="356" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A356" s="8"/>
     </row>
-    <row r="357" spans="1:1" ht="20.100000000000001">
+    <row r="357" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A357" s="8"/>
     </row>
-    <row r="358" spans="1:1" ht="20.100000000000001">
+    <row r="358" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A358" s="8"/>
     </row>
-    <row r="359" spans="1:1" ht="20.100000000000001">
+    <row r="359" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A359" s="8"/>
     </row>
-    <row r="360" spans="1:1" ht="20.100000000000001">
+    <row r="360" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A360" s="8"/>
     </row>
-    <row r="361" spans="1:1" ht="20.100000000000001">
+    <row r="361" spans="1:1" ht="20" x14ac:dyDescent="0.2">
       <c r="A361" s="8"/>
     </row>
   </sheetData>
@@ -4440,12 +4387,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f006263b-6855-4f81-be49-4241caee7f23">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="dabe3c20-206e-48c2-bf8d-a29783c980eb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4672,24 +4621,48 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f006263b-6855-4f81-be49-4241caee7f23">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="dabe3c20-206e-48c2-bf8d-a29783c980eb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65EBFEDB-1F62-4F1C-B496-B4021A8B8AE1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C683F71-BAD6-45A7-9C46-62C2D2F63BFF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f006263b-6855-4f81-be49-4241caee7f23"/>
+    <ds:schemaRef ds:uri="dabe3c20-206e-48c2-bf8d-a29783c980eb"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB92CAC3-9F74-4995-820F-13C750327611}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB92CAC3-9F74-4995-820F-13C750327611}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f006263b-6855-4f81-be49-4241caee7f23"/>
+    <ds:schemaRef ds:uri="dabe3c20-206e-48c2-bf8d-a29783c980eb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C683F71-BAD6-45A7-9C46-62C2D2F63BFF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{65EBFEDB-1F62-4F1C-B496-B4021A8B8AE1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>